<commit_message>
Added more QOL updates
</commit_message>
<xml_diff>
--- a/static/documents/asp_portfolio.xlsx
+++ b/static/documents/asp_portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agasthya\Desktop\ASP\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A799183-E61A-4CAE-8478-26857CD12C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CE34DE-6CA3-4A86-8CD9-8DA924AB02F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Company Name</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>09/09/24</t>
+  </si>
+  <si>
+    <t>Configs -------&gt;</t>
+  </si>
+  <si>
+    <t>Hit-T1</t>
+  </si>
+  <si>
+    <t>Hit-T2</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -135,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -165,11 +177,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -203,6 +226,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -510,10 +536,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,9 +555,10 @@
     <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,8 +598,17 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -604,8 +640,17 @@
       <c r="M2" s="6">
         <v>325.07</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -637,8 +682,17 @@
       <c r="M3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -665,41 +719,50 @@
       <c r="M4" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="12:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Friday Stop Loss Raise #1
</commit_message>
<xml_diff>
--- a/static/documents/asp_portfolio.xlsx
+++ b/static/documents/asp_portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agasthya\Desktop\ASP\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94580A72-7C47-49F7-ACD8-93DCD6F86286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CDC1F7-C34B-4E2C-986C-6E9F4C47BB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
         <v>18</v>
       </c>
       <c r="M3" s="8">
-        <v>0</v>
+        <v>97.11</v>
       </c>
       <c r="N3" t="s">
         <v>25</v>
@@ -776,7 +776,7 @@
         <v>28</v>
       </c>
       <c r="M5" s="8">
-        <v>0</v>
+        <v>66.790000000000006</v>
       </c>
       <c r="N5" t="s">
         <v>25</v>
@@ -811,7 +811,7 @@
         <v>28</v>
       </c>
       <c r="M6" s="8">
-        <v>43.11</v>
+        <v>45.55</v>
       </c>
       <c r="N6" t="s">
         <v>25</v>
@@ -840,7 +840,7 @@
         <v>57.17</v>
       </c>
       <c r="G7" s="8">
-        <v>65.209999999999994</v>
+        <v>67.069999999999993</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>33</v>
@@ -908,6 +908,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="L4" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Tesla + Performance Updates
</commit_message>
<xml_diff>
--- a/static/documents/asp_portfolio.xlsx
+++ b/static/documents/asp_portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agasthya\Desktop\ASP\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B66B775-3976-4AAF-88A9-B7B63B6CFE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA30EEDE-76D8-487A-9EF3-C163CFB0E540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Company Name</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>09/21/24</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>10/23/24</t>
   </si>
 </sst>
 </file>
@@ -554,7 +563,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,7 +822,39 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L7" s="9"/>
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8">
+        <v>216.58</v>
+      </c>
+      <c r="E7" s="8">
+        <v>205.22</v>
+      </c>
+      <c r="F7" s="8">
+        <v>239.1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>280.12</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="8">
+        <v>216.29</v>
+      </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L8" s="9"/>

</xml_diff>